<commit_message>
update template import and update done import
</commit_message>
<xml_diff>
--- a/public/template/import-participant.xlsx
+++ b/public/template/import-participant.xlsx
@@ -52,6 +52,9 @@
     <t>Tanggal kembali</t>
   </si>
   <si>
+    <t>#Note:</t>
+  </si>
+  <si>
     <t>Example</t>
   </si>
   <si>
@@ -71,9 +74,6 @@
   </si>
   <si>
     <t>Hotel Kita</t>
-  </si>
-  <si>
-    <t>#Note:</t>
   </si>
   <si>
     <t>Jangan diubah format maupun nama dan susunan columnya</t>
@@ -84,10 +84,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
   <fonts count="23">
@@ -129,14 +129,68 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -150,6 +204,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -158,9 +220,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -168,66 +236,13 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -237,21 +252,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,25 +273,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -303,157 +447,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -486,6 +486,17 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -506,6 +517,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -517,6 +537,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -539,43 +574,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -584,152 +584,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -750,6 +750,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1"/>
   </cellXfs>
@@ -1086,7 +1089,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5"/>
@@ -1119,7 +1122,7 @@
       <c r="J1" s="3"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:15">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1153,8 +1156,13 @@
       <c r="K2" s="6" t="s">
         <v>11</v>
       </c>
+      <c r="M2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1162,60 +1170,55 @@
         <v>45155</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="9" t="s">
         <v>15</v>
       </c>
+      <c r="F3" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" s="2">
         <v>45170</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K3" s="2">
         <v>45175</v>
       </c>
-      <c r="M3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
+      <c r="M3" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" spans="13:15">
-      <c r="M4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
     </row>
     <row r="5" spans="13:15">
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
     </row>
     <row r="6" spans="13:15">
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="M4:O6"/>
+    <mergeCell ref="M2:O2"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:E2">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>

</xml_diff>